<commit_message>
- Updated 808BD Host BOM - v1.0 PCB sent to OSHPark
</commit_message>
<xml_diff>
--- a/808bd/bom/808bd-host-bom.xlsx
+++ b/808bd/bom/808bd-host-bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="25040" yWindow="5420" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>5 x 2 pin 2.54mm pitch male header</t>
   </si>
   <si>
-    <t>517-929667-01-05-EU</t>
-  </si>
-  <si>
     <t>808 Bass Drum Host PCB BOM</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>pots to main pcb</t>
+  </si>
+  <si>
+    <t>649-68602-110HLF</t>
   </si>
 </sst>
 </file>
@@ -150,8 +150,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -162,9 +168,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -497,7 +509,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -509,7 +521,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="25">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16">
@@ -534,7 +546,7 @@
     </row>
     <row r="5" spans="1:4" ht="16">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -543,7 +555,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16">
@@ -557,7 +569,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16">
@@ -571,7 +583,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16">
@@ -589,7 +601,7 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16">
@@ -601,7 +613,7 @@
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16">
@@ -623,11 +635,11 @@
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>12</v>
+      <c r="C13" t="s">
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>